<commit_message>
NumMethods: continued lw 9
</commit_message>
<xml_diff>
--- a/Numerical methods/LW9/LW9.xlsx
+++ b/Numerical methods/LW9/LW9.xlsx
@@ -1,59 +1,69 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\studies\Numerical methods\LW9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\studies\Numerical methods\LW9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05266F85-ADCD-4943-990E-36D1C9956478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F53C24E-6EF2-493D-9467-42D8A406D20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>-4.7141        5.7974        0.8111       -1.0445        7.1756      -39.0244</t>
+    <t>x4</t>
   </si>
   <si>
-    <t xml:space="preserve">       -1.6180       -0.7646        4.5400       -5.7064       -4.2014       43.5179</t>
+    <t>x5</t>
+  </si>
+  <si>
+    <t>Исходная матрица</t>
+  </si>
+  <si>
+    <t>Преобразованная матрица</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,11 +86,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -361,65 +372,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G6"/>
+  <dimension ref="A2:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="8.1796875" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>-4.7141000000000002</v>
+      </c>
+      <c r="C3">
+        <v>5.7973999999999997</v>
+      </c>
+      <c r="D3">
+        <v>0.81110000000000004</v>
+      </c>
+      <c r="E3">
+        <v>-1.0445</v>
+      </c>
+      <c r="F3">
+        <v>7.1756000000000002</v>
+      </c>
+      <c r="G3">
+        <v>-39.0244</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>-4.7141000000000002</v>
-      </c>
-      <c r="C5">
-        <v>5.7973999999999997</v>
-      </c>
-      <c r="D5">
-        <v>0.81110000000000004</v>
-      </c>
-      <c r="E5">
-        <v>-1.0445</v>
-      </c>
-      <c r="F5">
-        <v>7.1756000000000002</v>
-      </c>
-      <c r="G5">
-        <v>-39.0244</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B4">
         <v>-1.6180000000000001</v>
       </c>
-      <c r="C6">
+      <c r="C4">
         <v>-0.76459999999999995</v>
       </c>
-      <c r="D6">
+      <c r="D4">
         <v>4.54</v>
       </c>
-      <c r="E6">
+      <c r="E4">
         <v>-5.7064000000000004</v>
       </c>
-      <c r="F6">
+      <c r="F4">
         <v>-4.2013999999999996</v>
       </c>
-      <c r="G6">
+      <c r="G4">
         <v>43.517899999999997</v>
       </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="I6" s="2">
+        <f>B10</f>
+        <v>-0.69298000000000004</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" ref="J6:K6" si="0">C10</f>
+        <v>0.41626999999999997</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.79378000000000004</v>
+      </c>
+      <c r="L6" s="2">
+        <f>G10</f>
+        <v>-3.2713999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>0.69298000000000004</v>
+      </c>
+      <c r="C7">
+        <v>-0.41626999999999997</v>
+      </c>
+      <c r="D7">
+        <v>-0.79378000000000004</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>-3.2713999999999999</v>
+      </c>
+      <c r="I7">
+        <f>B11</f>
+        <v>0.55608999999999997</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:K7" si="1">C11</f>
+        <v>-0.74734</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>2.5100000000000001E-3</v>
+      </c>
+      <c r="L7" s="2">
+        <f>G11</f>
+        <v>-5.9146799999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>-0.55608999999999997</v>
+      </c>
+      <c r="C8">
+        <v>0.74734</v>
+      </c>
+      <c r="D8">
+        <v>-2.5100000000000001E-3</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>-5.9146799999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <f>-B7</f>
+        <v>-0.69298000000000004</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:D10" si="2">-C7</f>
+        <v>0.41626999999999997</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0.79378000000000004</v>
+      </c>
+      <c r="G10">
+        <f>G7</f>
+        <v>-3.2713999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <f>-B8</f>
+        <v>0.55608999999999997</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="3">-C8</f>
+        <v>-0.74734</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>2.5100000000000001E-3</v>
+      </c>
+      <c r="G11">
+        <f>G8</f>
+        <v>-5.9146799999999997</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="I2:L2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>